<commit_message>
Streamlined the excel file Updated unit test
</commit_message>
<xml_diff>
--- a/Faez.BudgetAssistant.Excel.UnitTests/Files/Budget.xlsx
+++ b/Faez.BudgetAssistant.Excel.UnitTests/Files/Budget.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faez/Dropbox/Apps/Faez.BudgetAssistant/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faez/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="1500" windowWidth="25880" windowHeight="14700" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="700" yWindow="580" windowWidth="25880" windowHeight="14700" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" r:id="rId1"/>
@@ -35,24 +35,50 @@
     <author>Faez Hasnan</author>
   </authors>
   <commentList>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>UK 1701.50
-Mary 200
-Airbnb 1641
-Deposit 30</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">UK 1701.50
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Mary 200
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Airbnb 1641
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Deposit 30</t>
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,6 +123,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Zoe 1177
 </t>
@@ -107,12 +134,13 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>UK 700</t>
         </r>
       </text>
     </comment>
-    <comment ref="M10" authorId="1" shapeId="0">
+    <comment ref="M11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0">
+    <comment ref="H17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -134,6 +162,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">LED GU10 141.75
 </t>
@@ -144,6 +173,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Honeywell Lyric T6 26.95
 </t>
@@ -154,6 +184,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Airasia 101.08
 </t>
@@ -164,6 +195,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Hornbach 634.29
 </t>
@@ -174,12 +206,13 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Pans 68.77</t>
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0">
+    <comment ref="I17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -187,6 +220,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Lights 80
 Kitchenaid 232.56
@@ -196,7 +230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0" shapeId="0">
+    <comment ref="J17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -204,6 +238,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Blokker 114.43
 </t>
@@ -214,6 +249,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Contact Lens 55.80
 </t>
@@ -224,6 +260,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Easyjet 72.67
 </t>
@@ -234,6 +271,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">London 96
 </t>
@@ -244,6 +282,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Ikea 97.87
 </t>
@@ -254,6 +293,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">KUL-KOS 61.63
 </t>
@@ -264,13 +304,14 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Zara 41.93
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="K16" authorId="0" shapeId="0">
+    <comment ref="K17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -278,12 +319,13 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>AMS-KUL 785.19</t>
         </r>
       </text>
     </comment>
-    <comment ref="M16" authorId="1" shapeId="0">
+    <comment ref="M17" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -291,12 +333,13 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Luminosity</t>
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0" shapeId="0">
+    <comment ref="H21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -304,13 +347,14 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Bartek P1 500
 Additional 2500</t>
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0">
+    <comment ref="I21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -318,6 +362,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Witek 198.20
 Bartek P1 1000
@@ -326,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0" shapeId="0">
+    <comment ref="K21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -334,6 +379,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Bartek P2 2000
 </t>
@@ -344,6 +390,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Materials 3000
 </t>
@@ -353,13 +400,14 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="L20" authorId="0" shapeId="0">
+    <comment ref="L21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -367,6 +415,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Bartek P2 1600
 </t>
@@ -377,6 +426,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -386,13 +436,14 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0" shapeId="0">
+    <comment ref="C22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -400,12 +451,13 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Council tax</t>
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0" shapeId="0">
+    <comment ref="F22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -413,6 +465,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Belastingdienst 283
 Belastingdienst 1541
@@ -425,7 +478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0" shapeId="0">
+    <comment ref="G22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -433,6 +486,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">House 11897.79
 AMS-KUL 1219.16
@@ -443,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H21" authorId="0" shapeId="0">
+    <comment ref="H22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -451,6 +505,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">HEMA 103.10
 </t>
@@ -461,6 +516,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Keys 17.10
 </t>
@@ -471,6 +527,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Supplements 39.30
 </t>
@@ -481,12 +538,13 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Deposit 100</t>
         </r>
       </text>
     </comment>
-    <comment ref="I21" authorId="1" shapeId="0">
+    <comment ref="I22" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -504,7 +562,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J21" authorId="0" shapeId="0">
+    <comment ref="J22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -512,6 +570,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Nederlands 1 390
 </t>
@@ -522,6 +581,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Book 39.50
 </t>
@@ -532,12 +592,13 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>NS 153</t>
         </r>
       </text>
     </comment>
-    <comment ref="K21" authorId="0" shapeId="0">
+    <comment ref="K22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -545,6 +606,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Lonely Planet 11.48
 </t>
@@ -555,6 +617,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Curtain 40
 </t>
@@ -565,12 +628,13 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Paris 161</t>
         </r>
       </text>
     </comment>
-    <comment ref="M21" authorId="1" shapeId="0">
+    <comment ref="M22" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -578,6 +642,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">VVE 297.50
 </t>
@@ -588,6 +653,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Body en Fit 61.18
 </t>
@@ -598,13 +664,14 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Nederlands 2A 351
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0">
+    <comment ref="F26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -629,7 +696,7 @@
     <author>Faez Hasnan</author>
   </authors>
   <commentList>
-    <comment ref="C20" authorId="0" shapeId="0">
+    <comment ref="C21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -637,6 +704,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Bartek P2 1500
 </t>
@@ -647,6 +715,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -656,13 +725,14 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0">
+    <comment ref="D21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -670,6 +740,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Bartek P2 1500
 </t>
@@ -680,6 +751,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -689,13 +761,14 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="1" shapeId="0">
+    <comment ref="B22" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -725,7 +798,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="41">
   <si>
     <t>October</t>
   </si>
@@ -846,6 +919,9 @@
   <si>
     <t>Internet + Spotify</t>
   </si>
+  <si>
+    <t>England</t>
+  </si>
 </sst>
 </file>
 
@@ -855,7 +931,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$MYR]\ * #,##0.00_);_([$MYR]\ * \(#,##0.00\);_([$MYR]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -918,20 +994,16 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -942,12 +1014,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1006,7 +1078,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="6"/>
@@ -1029,6 +1101,7 @@
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -1340,10 +1413,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1382,174 +1455,173 @@
         <v>3559.2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6">
-        <f>691.64+B23</f>
-        <v>5691.64</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="6">
+        <v>691.64</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1065</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1190</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1190</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1065</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1190</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B9" s="8">
         <v>101.14</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C9" s="8">
         <v>101.14</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D9" s="8">
         <v>101.14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B10" s="8">
         <v>22.01</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C10" s="8">
         <v>22</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D10" s="8">
         <v>20.49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="8">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="8">
-        <v>0</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="8">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8">
         <v>7.83</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D13" s="8">
         <v>7.83</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-    </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B15" s="9">
         <v>80</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C15" s="9">
         <v>80</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D15" s="9">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B16" s="9">
         <v>150</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C16" s="9">
         <v>52</v>
       </c>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="9">
-        <v>1189.58</v>
-      </c>
-      <c r="C16" s="9">
-        <v>717.61</v>
-      </c>
       <c r="D16" s="9">
-        <v>890.99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B17" s="9">
-        <v>0</v>
+        <v>1189.58</v>
       </c>
       <c r="C17" s="9">
-        <v>0</v>
+        <v>717.61</v>
       </c>
       <c r="D17" s="9">
-        <v>0</v>
+        <v>890.99</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="9">
         <v>0</v>
@@ -1563,188 +1635,201 @@
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B19" s="9">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C19" s="9">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D19" s="9">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="9">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="C20" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D20" s="9">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="A21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="9">
+        <v>400</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>100</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B23" s="9">
         <v>1000</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C23" s="9">
         <v>1000</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D23" s="9">
         <v>1500</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="9">
-        <v>5000</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B25" s="9">
         <v>4725.0600000000004</v>
       </c>
-      <c r="C24" s="9">
-        <v>0</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B26" s="11">
         <v>50.21</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C26" s="11">
         <v>19.829999999999998</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D26" s="11">
         <v>8.36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-    </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="10">
-        <f>SUM(B4:B5)-SUM(B7:B12)-SUM(B14:B20)-SUM(B22:B25)+B23</f>
-        <v>367.84000000000015</v>
-      </c>
-      <c r="C27" s="10">
-        <f>SUM(C4:C5)-SUM(C7:C12)-SUM(C14:C20)-SUM(C22:C25)+B27+C23</f>
-        <v>636.62999999999954</v>
-      </c>
-      <c r="D27" s="10">
-        <f t="shared" ref="D27" si="0">SUM(D4:D5)-SUM(D7:D12)-SUM(D14:D20)-SUM(D22:D25)+C27+D23</f>
-        <v>197.01999999999941</v>
-      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="10">
+        <f>SUM(B4:B6)-SUM(B8:B13)-SUM(B15:B21)-SUM(B23:B26)</f>
+        <v>367.84000000000015</v>
+      </c>
+      <c r="C28" s="10">
+        <f>SUM(C4:C6)-SUM(C8:C13)-SUM(C15:C21)-SUM(C23:C26)+B28</f>
+        <v>636.62999999999954</v>
+      </c>
+      <c r="D28" s="10">
+        <f>SUM(D4:D6)-SUM(D8:D13)-SUM(D15:D21)-SUM(D23:D26)+C28</f>
+        <v>197.01999999999941</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="13">
-        <f>B22-B23+7000</f>
+      <c r="B29" s="13">
         <v>3000</v>
       </c>
-      <c r="C28" s="13">
-        <f>C22+B28</f>
+      <c r="C29" s="13">
+        <f>C23+B29</f>
         <v>4000</v>
       </c>
-      <c r="D28" s="13">
-        <f>D22+C28</f>
+      <c r="D29" s="13">
+        <f>D23+C29</f>
         <v>5500</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="10">
-        <f>B27+B28</f>
+      <c r="B30" s="10">
+        <f>B28+B29</f>
         <v>3367.84</v>
       </c>
-      <c r="C29" s="10">
-        <f t="shared" ref="C29:D29" si="1">C27+C28</f>
+      <c r="C30" s="10">
+        <f t="shared" ref="C30:D30" si="0">C28+C29</f>
         <v>4636.6299999999992</v>
       </c>
-      <c r="D29" s="10">
-        <f t="shared" si="1"/>
+      <c r="D30" s="10">
+        <f t="shared" si="0"/>
         <v>5697.0199999999995</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="17">
-        <v>233958.5</v>
-      </c>
-      <c r="C31" s="17">
-        <v>233958.5</v>
-      </c>
-      <c r="D31" s="17">
-        <v>233958.5</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="17">
-        <v>200000</v>
+        <v>233958.5</v>
       </c>
       <c r="C32" s="17">
-        <v>200000</v>
+        <v>233958.5</v>
       </c>
       <c r="D32" s="17">
-        <v>200000</v>
+        <v>233958.5</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="17">
+        <v>200000</v>
+      </c>
+      <c r="C33" s="17">
+        <v>200000</v>
+      </c>
+      <c r="D33" s="17">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B34" s="17">
         <v>49787.13</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C34" s="17">
         <v>92466.66</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D34" s="17">
         <v>92466.66</v>
       </c>
     </row>
@@ -1752,9 +1837,6 @@
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="C27" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1763,10 +1845,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1859,497 +1941,497 @@
         <v>4019.58</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
         <v>32348.28</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E6" s="6">
         <v>120</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F6" s="18">
         <v>1459.13</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G6" s="6">
         <v>30000</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H6" s="6">
         <v>4072.5</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I6" s="6">
         <v>1499.97</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J6" s="6">
         <v>2116.21</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K6" s="6">
         <v>4400</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L6" s="6">
         <v>6148.43</v>
       </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1165</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1190</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1190</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1190</v>
-      </c>
-      <c r="F7" s="8">
-        <v>1190</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1190</v>
-      </c>
-      <c r="H7" s="8">
-        <v>2305.92</v>
-      </c>
-      <c r="I7" s="8">
-        <v>1099</v>
-      </c>
-      <c r="J7" s="8">
-        <v>1099</v>
-      </c>
-      <c r="K7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="L7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="M7" s="8">
-        <v>1097.43</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1165</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1190</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1190</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1190</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1190</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1190</v>
+      </c>
+      <c r="H8" s="8">
+        <v>2305.92</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1099</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1099</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1097.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B9" s="8">
         <v>104.55</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C9" s="8">
         <v>104.55</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D9" s="8">
         <v>104.55</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E9" s="8">
         <v>104.55</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F9" s="8">
         <v>104.55</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G9" s="8">
         <v>104.55</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H9" s="8">
         <v>111.74</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I9" s="8">
         <v>111.74</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J9" s="8">
         <v>111.74</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K9" s="8">
         <v>111.74</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L9" s="8">
         <v>111.74</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M9" s="8">
         <v>111.74</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B10" s="8">
         <v>22.46</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C10" s="8">
         <v>15.27</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D10" s="8">
         <v>17.98</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E10" s="8">
         <v>17.98</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F10" s="8">
         <v>18.23</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G10" s="8">
         <v>17.98</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H10" s="8">
         <v>20.51</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I10" s="8">
         <v>21.64</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J10" s="8">
         <v>24.79</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K10" s="8">
         <v>17.98</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L10" s="8">
         <v>17.98</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M10" s="8">
         <v>17.98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="8">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8">
-        <v>29.95</v>
-      </c>
-      <c r="H10" s="8">
-        <v>39.94</v>
-      </c>
-      <c r="I10" s="8">
-        <v>39.94</v>
-      </c>
-      <c r="J10" s="8">
-        <v>39.94</v>
-      </c>
-      <c r="K10" s="8">
-        <v>39.94</v>
-      </c>
-      <c r="L10" s="8">
-        <v>39.94</v>
-      </c>
-      <c r="M10" s="8">
-        <v>129.94</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>29.95</v>
+      </c>
+      <c r="H11" s="8">
+        <v>39.94</v>
+      </c>
+      <c r="I11" s="8">
+        <v>39.94</v>
+      </c>
+      <c r="J11" s="8">
+        <v>39.94</v>
+      </c>
+      <c r="K11" s="8">
+        <v>39.94</v>
+      </c>
+      <c r="L11" s="8">
+        <v>39.94</v>
+      </c>
+      <c r="M11" s="8">
+        <v>129.94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="8">
-        <v>0</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
         <v>88</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H12" s="8">
         <v>88</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I12" s="8">
         <v>88</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J12" s="8">
         <v>88</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K12" s="8">
         <v>78</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L12" s="8">
         <v>78</v>
       </c>
-      <c r="M11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="M12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B13" s="8">
         <v>7.83</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C13" s="8">
         <v>7.83</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D13" s="8">
         <v>7.83</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E13" s="8">
         <v>41.12</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F13" s="8">
         <v>41.12</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G13" s="8">
         <v>41.12</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H13" s="8">
         <v>41.12</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I13" s="8">
         <v>41.12</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J13" s="8">
         <v>41.12</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K13" s="8">
         <v>41.12</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L13" s="8">
         <v>41.12</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M13" s="8">
         <v>41.12</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-    </row>
     <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B15" s="9">
         <v>80</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C15" s="9">
         <v>80</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D15" s="9">
         <v>80</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E15" s="9">
         <v>120</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F15" s="9">
         <v>120</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G15" s="9">
         <v>120</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H15" s="9">
         <v>170</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I15" s="9">
         <v>120</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J15" s="9">
         <v>120</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K15" s="9">
         <v>120</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L15" s="9">
         <v>50</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M15" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>0</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-      <c r="E15" s="9">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
         <v>90</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H16" s="9">
         <v>165</v>
       </c>
-      <c r="I15" s="9">
-        <v>0</v>
-      </c>
-      <c r="J15" s="9">
+      <c r="I16" s="9">
+        <v>0</v>
+      </c>
+      <c r="J16" s="9">
         <v>140</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K16" s="9">
         <v>186</v>
       </c>
-      <c r="L15" s="9">
-        <v>0</v>
-      </c>
-      <c r="M15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="9">
-        <v>173.49</v>
-      </c>
-      <c r="C16" s="9">
-        <v>780.98</v>
-      </c>
-      <c r="D16" s="9">
-        <v>407.26</v>
-      </c>
-      <c r="E16" s="9">
-        <v>9.99</v>
-      </c>
-      <c r="F16" s="9">
-        <v>59.64</v>
-      </c>
-      <c r="G16" s="9">
-        <v>437.26</v>
-      </c>
-      <c r="H16" s="9">
-        <v>942.41</v>
-      </c>
-      <c r="I16" s="9">
-        <v>1306.52</v>
-      </c>
-      <c r="J16" s="9">
-        <v>537.29</v>
-      </c>
-      <c r="K16" s="9">
-        <v>1046.1500000000001</v>
-      </c>
       <c r="L16" s="9">
-        <v>499.42</v>
+        <v>0</v>
       </c>
       <c r="M16" s="9">
-        <v>367.54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B17" s="9">
-        <v>50</v>
+        <v>173.49</v>
       </c>
       <c r="C17" s="9">
-        <v>0</v>
+        <v>780.98</v>
       </c>
       <c r="D17" s="9">
-        <v>110</v>
+        <v>407.26</v>
       </c>
       <c r="E17" s="9">
-        <v>0</v>
+        <v>9.99</v>
       </c>
       <c r="F17" s="9">
-        <v>0</v>
+        <v>59.64</v>
       </c>
       <c r="G17" s="9">
-        <v>117.58</v>
+        <v>437.26</v>
       </c>
       <c r="H17" s="9">
-        <v>0</v>
+        <v>942.41</v>
       </c>
       <c r="I17" s="9">
-        <v>80</v>
+        <v>1306.52</v>
       </c>
       <c r="J17" s="9">
-        <v>0</v>
+        <v>537.29</v>
       </c>
       <c r="K17" s="9">
-        <v>0</v>
+        <v>1046.1500000000001</v>
       </c>
       <c r="L17" s="9">
-        <v>0</v>
+        <v>499.42</v>
       </c>
       <c r="M17" s="9">
-        <v>0</v>
+        <v>367.54</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="9">
-        <v>718.06</v>
+        <v>50</v>
       </c>
       <c r="C18" s="9">
         <v>0</v>
       </c>
       <c r="D18" s="9">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E18" s="9">
         <v>0</v>
@@ -2358,13 +2440,13 @@
         <v>0</v>
       </c>
       <c r="G18" s="9">
-        <v>0</v>
+        <v>117.58</v>
       </c>
       <c r="H18" s="9">
         <v>0</v>
       </c>
       <c r="I18" s="9">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J18" s="9">
         <v>0</v>
@@ -2376,603 +2458,644 @@
         <v>0</v>
       </c>
       <c r="M18" s="9">
-        <v>718.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="9">
+        <v>718.06</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0</v>
+      </c>
+      <c r="M19" s="9">
+        <v>718.95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B20" s="9">
         <v>150</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C20" s="9">
         <v>100</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D20" s="9">
         <v>100</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E20" s="9">
         <v>126</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F20" s="9">
         <v>100</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G20" s="9">
         <v>250</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H20" s="9">
         <v>210</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I20" s="9">
         <v>100</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J20" s="9">
         <v>100</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K20" s="9">
         <v>250</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L20" s="9">
         <v>100</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M20" s="9">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="9">
-        <v>0</v>
-      </c>
-      <c r="C20" s="9">
-        <v>0</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0</v>
-      </c>
-      <c r="E20" s="9">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0</v>
-      </c>
-      <c r="G20" s="9">
-        <v>0</v>
-      </c>
-      <c r="H20" s="9">
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
         <v>3000</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I21" s="9">
         <v>1498.2</v>
       </c>
-      <c r="J20" s="9">
-        <v>0</v>
-      </c>
-      <c r="K20" s="9">
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
         <v>5000</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L21" s="9">
         <v>1600</v>
       </c>
-      <c r="M20" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B22" s="9">
         <v>150</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C22" s="9">
         <v>363</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D22" s="9">
         <v>63.75</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E22" s="9">
         <v>21.7</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F22" s="9">
         <v>2615.54</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G22" s="19">
         <v>18125.8</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H22" s="9">
         <v>259.5</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I22" s="9">
         <v>810.69</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J22" s="9">
         <v>582.5</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K22" s="9">
         <v>212.48</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L22" s="9">
         <v>22.5</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M22" s="9">
         <v>709.68</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-    </row>
     <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B24" s="9">
         <v>2500</v>
       </c>
-      <c r="C23" s="9">
-        <v>0</v>
-      </c>
-      <c r="D23" s="9">
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
         <v>34000</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E24" s="9">
         <v>2750</v>
       </c>
-      <c r="F23" s="9">
-        <v>0</v>
-      </c>
-      <c r="G23" s="9">
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
         <v>711.31</v>
       </c>
-      <c r="H23" s="9">
-        <v>0</v>
-      </c>
-      <c r="I23" s="9">
+      <c r="H24" s="9">
+        <v>0</v>
+      </c>
+      <c r="I24" s="9">
         <v>700</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J24" s="9">
         <v>400</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K24" s="9">
         <v>600</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L24" s="9">
         <v>500</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M24" s="9">
         <v>500</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="9">
-        <v>0</v>
-      </c>
-      <c r="C24" s="9">
-        <v>1200</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0</v>
-      </c>
-      <c r="F24" s="9">
-        <v>1461.31</v>
-      </c>
-      <c r="G24" s="9">
-        <v>30000</v>
-      </c>
-      <c r="H24" s="9">
-        <v>500</v>
-      </c>
-      <c r="I24" s="9">
-        <v>0</v>
-      </c>
-      <c r="J24" s="9">
-        <v>200</v>
-      </c>
-      <c r="K24" s="9">
-        <v>4400</v>
-      </c>
-      <c r="L24" s="9">
-        <v>6100</v>
-      </c>
-      <c r="M24" s="9">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="9">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9">
+      <c r="B26" s="9">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9">
         <v>1200</v>
       </c>
-      <c r="D25" s="9">
-        <v>0</v>
-      </c>
-      <c r="E25" s="9">
-        <v>0</v>
-      </c>
-      <c r="F25" s="9">
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9">
         <v>1298.72</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G26" s="9">
         <v>12500</v>
       </c>
-      <c r="H25" s="9">
-        <v>0</v>
-      </c>
-      <c r="I25" s="9">
-        <v>0</v>
-      </c>
-      <c r="J25" s="9">
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0</v>
+      </c>
+      <c r="J26" s="9">
         <v>2610</v>
       </c>
-      <c r="K25" s="9">
-        <v>0</v>
-      </c>
-      <c r="L25" s="9">
+      <c r="K26" s="9">
+        <v>0</v>
+      </c>
+      <c r="L26" s="9">
         <v>6011.07</v>
       </c>
-      <c r="M25" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="M26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B27" s="11">
         <v>33.32</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C27" s="11">
         <v>50</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D27" s="11">
         <v>70.849999999999994</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E27" s="11">
         <v>77.36</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F27" s="11">
         <v>47.85</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G27" s="11">
         <v>51.2</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H27" s="11">
         <v>141.36000000000001</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I27" s="11">
         <v>55.96</v>
       </c>
-      <c r="J26" s="11">
-        <v>0</v>
-      </c>
-      <c r="K26" s="11">
+      <c r="J27" s="11">
+        <v>0</v>
+      </c>
+      <c r="K27" s="11">
         <v>25.63</v>
       </c>
-      <c r="L26" s="11">
-        <v>0</v>
-      </c>
-      <c r="M26" s="11">
+      <c r="L27" s="11">
+        <v>0</v>
+      </c>
+      <c r="M27" s="11">
         <v>30.05</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-    </row>
     <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="10">
-        <f>SUM(B4:B5)-SUM(B7:B12)-SUM(B14:B21)-SUM(B23:B26)+B24+'2016'!D27</f>
+      <c r="B29" s="10">
+        <f>SUM(B4:B6)-SUM(B8:B13)-SUM(B15:B22)-SUM(B24:B27)+'2016'!D28</f>
         <v>202.14999999999907</v>
       </c>
-      <c r="C28" s="10">
-        <f t="shared" ref="C28:M28" si="0">SUM(C4:C5)-SUM(C7:C12)-SUM(C14:C21)-SUM(C23:C26)+B28+C24</f>
+      <c r="C29" s="10">
+        <f>SUM(C4:C6)-SUM(C8:C13)-SUM(C15:C22)-SUM(C24:C27)+B29</f>
         <v>346.59999999999934</v>
       </c>
-      <c r="D28" s="10">
-        <f t="shared" si="0"/>
+      <c r="D29" s="10">
+        <f t="shared" ref="D29:M29" si="0">SUM(D4:D6)-SUM(D8:D13)-SUM(D15:D22)-SUM(D24:D27)+C29</f>
         <v>578.73999999999876</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E29" s="10">
         <f t="shared" si="0"/>
         <v>276.11999999999887</v>
       </c>
-      <c r="F28" s="10">
-        <f>SUM(F4:F5)-SUM(F7:F12)-SUM(F14:F21)-SUM(F23:F26)+E28+F24</f>
-        <v>175.67999999999984</v>
-      </c>
-      <c r="G28" s="10">
+      <c r="F29" s="10">
         <f t="shared" si="0"/>
-        <v>337.01000000000931</v>
-      </c>
-      <c r="H28" s="10">
-        <f>SUM(H4:H5)-SUM(H7:H12)-SUM(H14:H21)-SUM(H23:H26)+G28+H24</f>
-        <v>950.09000000000981</v>
-      </c>
-      <c r="I28" s="10">
-        <f>SUM(I4:I5)-SUM(I7:I12)-SUM(I14:I21)-SUM(I23:I26)+H28+I24</f>
-        <v>413.33000000001005</v>
-      </c>
-      <c r="J28" s="10">
-        <f>SUM(J4:J5)-SUM(J7:J12)-SUM(J14:J21)-SUM(J23:J26)+I28+J24</f>
-        <v>671.2400000000099</v>
-      </c>
-      <c r="K28" s="10">
+        <v>175.6799999999995</v>
+      </c>
+      <c r="G29" s="10">
         <f t="shared" si="0"/>
-        <v>244.5500000000111</v>
-      </c>
-      <c r="L28" s="10">
+        <v>337.01000000000306</v>
+      </c>
+      <c r="H29" s="10">
         <f t="shared" si="0"/>
-        <v>223.56000000001131</v>
-      </c>
-      <c r="M28" s="10">
+        <v>950.09000000000356</v>
+      </c>
+      <c r="I29" s="10">
         <f t="shared" si="0"/>
-        <v>298.71000000001118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
+        <v>413.33000000000379</v>
+      </c>
+      <c r="J29" s="10">
+        <f t="shared" si="0"/>
+        <v>671.24000000000365</v>
+      </c>
+      <c r="K29" s="10">
+        <f t="shared" si="0"/>
+        <v>244.55000000000507</v>
+      </c>
+      <c r="L29" s="10">
+        <f t="shared" si="0"/>
+        <v>223.56000000000529</v>
+      </c>
+      <c r="M29" s="10">
+        <f t="shared" si="0"/>
+        <v>298.71000000000515</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="13">
-        <f>B23+'2016'!D28</f>
+      <c r="B30" s="13">
+        <f>B24+'2016'!D29</f>
         <v>8000</v>
       </c>
-      <c r="C29" s="13">
-        <f t="shared" ref="C29:E29" si="1">C23+B29</f>
+      <c r="C30" s="13">
+        <f t="shared" ref="C30:E30" si="1">C24+B30</f>
         <v>8000</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D30" s="13">
         <f t="shared" si="1"/>
         <v>42000</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E30" s="13">
         <f t="shared" si="1"/>
         <v>44750</v>
       </c>
-      <c r="F29" s="13">
-        <f>F23+E29-F24</f>
-        <v>43288.69</v>
-      </c>
-      <c r="G29" s="13">
-        <f>G23+F29-G24</f>
-        <v>14000</v>
-      </c>
-      <c r="H29" s="13">
-        <f>H23+G29-H24</f>
-        <v>13500</v>
-      </c>
-      <c r="I29" s="13">
-        <f t="shared" ref="I29:M29" si="2">I23+H29-I24</f>
-        <v>14200</v>
-      </c>
-      <c r="J29" s="13">
+      <c r="F30" s="13">
+        <f>F24+E30-F25</f>
+        <v>44750</v>
+      </c>
+      <c r="G30" s="13">
+        <f>G24+F30-G25</f>
+        <v>45461.31</v>
+      </c>
+      <c r="H30" s="13">
+        <f>H24+G30-H25</f>
+        <v>45461.31</v>
+      </c>
+      <c r="I30" s="13">
+        <f t="shared" ref="I30:M30" si="2">I24+H30-I25</f>
+        <v>46161.31</v>
+      </c>
+      <c r="J30" s="13">
         <f t="shared" si="2"/>
-        <v>14400</v>
-      </c>
-      <c r="K29" s="13">
+        <v>46561.31</v>
+      </c>
+      <c r="K30" s="13">
         <f t="shared" si="2"/>
-        <v>10600</v>
-      </c>
-      <c r="L29" s="13">
+        <v>47161.31</v>
+      </c>
+      <c r="L30" s="13">
         <f t="shared" si="2"/>
-        <v>5000</v>
-      </c>
-      <c r="M29" s="13">
+        <v>47661.31</v>
+      </c>
+      <c r="M30" s="13">
         <f t="shared" si="2"/>
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+        <v>48161.31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="10">
-        <f t="shared" ref="B30:M30" si="3">B28+B29</f>
+      <c r="B31" s="10">
+        <f t="shared" ref="B31:M31" si="3">B29+B30</f>
         <v>8202.15</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C31" s="10">
         <f t="shared" si="3"/>
         <v>8346.5999999999985</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D31" s="10">
         <f t="shared" si="3"/>
         <v>42578.74</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E31" s="10">
         <f t="shared" si="3"/>
         <v>45026.119999999995</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F31" s="10">
         <f t="shared" si="3"/>
-        <v>43464.37</v>
-      </c>
-      <c r="G30" s="10">
+        <v>44925.68</v>
+      </c>
+      <c r="G31" s="10">
         <f t="shared" si="3"/>
-        <v>14337.010000000009</v>
-      </c>
-      <c r="H30" s="10">
+        <v>45798.32</v>
+      </c>
+      <c r="H31" s="10">
         <f t="shared" si="3"/>
-        <v>14450.090000000009</v>
-      </c>
-      <c r="I30" s="10">
+        <v>46411.4</v>
+      </c>
+      <c r="I31" s="10">
         <f t="shared" si="3"/>
-        <v>14613.330000000011</v>
-      </c>
-      <c r="J30" s="10">
+        <v>46574.64</v>
+      </c>
+      <c r="J31" s="10">
         <f t="shared" si="3"/>
-        <v>15071.240000000011</v>
-      </c>
-      <c r="K30" s="10">
+        <v>47232.55</v>
+      </c>
+      <c r="K31" s="10">
         <f t="shared" si="3"/>
-        <v>10844.55000000001</v>
-      </c>
-      <c r="L30" s="10">
+        <v>47405.86</v>
+      </c>
+      <c r="L31" s="10">
         <f t="shared" si="3"/>
-        <v>5223.5600000000113</v>
-      </c>
-      <c r="M30" s="10">
+        <v>47884.87</v>
+      </c>
+      <c r="M31" s="10">
         <f t="shared" si="3"/>
-        <v>5798.710000000011</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="C32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="D32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="E32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="F32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="G32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="H32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="I32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="J32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="K32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="L32" s="17">
-        <v>250360.35</v>
-      </c>
-      <c r="M32" s="17">
-        <v>250360.35</v>
+        <v>48460.020000000004</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="17">
-        <v>200000</v>
+        <v>250360.35</v>
       </c>
       <c r="C33" s="17">
-        <v>200000</v>
+        <v>250360.35</v>
       </c>
       <c r="D33" s="17">
-        <v>200000</v>
+        <v>250360.35</v>
       </c>
       <c r="E33" s="17">
-        <v>212208.55</v>
+        <v>250360.35</v>
       </c>
       <c r="F33" s="17">
-        <v>212208.55</v>
+        <v>250360.35</v>
       </c>
       <c r="G33" s="17">
-        <v>212208.55</v>
+        <v>250360.35</v>
       </c>
       <c r="H33" s="17">
-        <v>212208.55</v>
+        <v>250360.35</v>
       </c>
       <c r="I33" s="17">
-        <v>212208.55</v>
+        <v>250360.35</v>
       </c>
       <c r="J33" s="17">
-        <v>212208.55</v>
+        <v>250360.35</v>
       </c>
       <c r="K33" s="17">
-        <v>212208.55</v>
+        <v>250360.35</v>
       </c>
       <c r="L33" s="17">
-        <v>212208.55</v>
+        <v>250360.35</v>
       </c>
       <c r="M33" s="17">
-        <v>212208.55</v>
+        <v>250360.35</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="17">
+        <v>200000</v>
+      </c>
+      <c r="C34" s="17">
+        <v>200000</v>
+      </c>
+      <c r="D34" s="17">
+        <v>200000</v>
+      </c>
+      <c r="E34" s="17">
+        <v>212208.55</v>
+      </c>
+      <c r="F34" s="17">
+        <v>212208.55</v>
+      </c>
+      <c r="G34" s="17">
+        <v>212208.55</v>
+      </c>
+      <c r="H34" s="17">
+        <v>212208.55</v>
+      </c>
+      <c r="I34" s="17">
+        <v>212208.55</v>
+      </c>
+      <c r="J34" s="17">
+        <v>212208.55</v>
+      </c>
+      <c r="K34" s="17">
+        <v>212208.55</v>
+      </c>
+      <c r="L34" s="17">
+        <v>212208.55</v>
+      </c>
+      <c r="M34" s="17">
+        <v>212208.55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B35" s="17">
         <v>92466.66</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C35" s="17">
         <v>92466.66</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D35" s="17">
         <v>87675.04</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E35" s="17">
         <v>87675.04</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F35" s="17">
         <v>87675.04</v>
       </c>
-      <c r="G34" s="17">
+      <c r="G35" s="17">
         <v>87675.04</v>
       </c>
-      <c r="H34" s="17">
+      <c r="H35" s="17">
         <v>131000</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I35" s="17">
         <v>131000</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J35" s="17">
         <v>131000</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K35" s="17">
         <v>135493</v>
       </c>
-      <c r="L34" s="17">
+      <c r="L35" s="17">
         <v>120493.32</v>
       </c>
-      <c r="M34" s="17">
+      <c r="M35" s="17">
         <v>150000.32000000001</v>
       </c>
     </row>
@@ -2988,10 +3111,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3084,456 +3207,456 @@
         <v>3999.78</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6">
-        <v>40</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
         <v>25000</v>
       </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="F7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="I7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="J7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="K7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="L7" s="8">
-        <v>1097.43</v>
-      </c>
-      <c r="M7" s="8">
-        <v>1097.43</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1097.43</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1097.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B9" s="8">
         <v>107.37</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C9" s="8">
         <v>107.37</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D9" s="8">
         <v>107.37</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E9" s="8">
         <v>107.37</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F9" s="8">
         <v>107.37</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G9" s="8">
         <v>107.37</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H9" s="8">
         <v>107.37</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I9" s="8">
         <v>107.37</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J9" s="8">
         <v>107.37</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K9" s="8">
         <v>107.37</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L9" s="8">
         <v>107.37</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M9" s="8">
         <v>107.37</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B10" s="8">
         <v>12.6</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C10" s="8">
         <v>13</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D10" s="8">
         <v>13</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E10" s="8">
         <v>13</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F10" s="8">
         <v>13</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G10" s="8">
         <v>13</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H10" s="8">
         <v>13</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I10" s="8">
         <v>13</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J10" s="8">
         <v>13</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K10" s="8">
         <v>13</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L10" s="8">
         <v>13</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M10" s="8">
         <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="C10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="D10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="E10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="F10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="G10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="H10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="I10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="J10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="K10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="L10" s="8">
-        <v>30.95</v>
-      </c>
-      <c r="M10" s="8">
-        <v>30.95</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="C11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="D11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="E11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="F11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="G11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="H11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="I11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="J11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="K11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="L11" s="8">
+        <v>30.95</v>
+      </c>
+      <c r="M11" s="8">
+        <v>30.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B12" s="8">
         <v>156</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C12" s="8">
         <v>78</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D12" s="8">
         <v>78</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E12" s="8">
         <v>78</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F12" s="8">
         <v>78</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G12" s="8">
         <v>78</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H12" s="8">
         <v>78</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I12" s="8">
         <v>78</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J12" s="8">
         <v>78</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K12" s="8">
         <v>78</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L12" s="8">
         <v>78</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M12" s="8">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B13" s="8">
         <v>41.12</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C13" s="8">
         <v>41.12</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D13" s="8">
         <v>41.12</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E13" s="8">
         <v>41.12</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F13" s="8">
         <v>41.12</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G13" s="8">
         <v>41.12</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H13" s="8">
         <v>41.12</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I13" s="8">
         <v>41.12</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J13" s="8">
         <v>41.12</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K13" s="8">
         <v>41.12</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L13" s="8">
         <v>41.12</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M13" s="8">
         <v>41.12</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-    </row>
     <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B15" s="9">
         <v>120</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C15" s="9">
         <v>120</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D15" s="9">
         <v>60</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E15" s="9">
         <v>120</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F15" s="9">
         <v>120</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G15" s="9">
         <v>120</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H15" s="9">
         <v>120</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I15" s="9">
         <v>120</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J15" s="9">
         <v>120</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K15" s="9">
         <v>120</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L15" s="9">
         <v>120</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M15" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B16" s="9">
         <v>45</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C16" s="9">
         <v>186</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D16" s="9">
         <v>186</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E16" s="9">
         <v>186</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F16" s="9">
         <v>186</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G16" s="9">
         <v>186</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H16" s="9">
         <v>186</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I16" s="9">
         <v>186</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J16" s="9">
         <v>186</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K16" s="9">
         <v>186</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L16" s="9">
         <v>186</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M16" s="9">
         <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="9">
-        <v>582.83000000000004</v>
-      </c>
-      <c r="C16" s="9">
-        <v>571.09</v>
-      </c>
-      <c r="D16" s="9">
-        <v>134.13</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0</v>
-      </c>
-      <c r="I16" s="9">
-        <v>0</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0</v>
-      </c>
-      <c r="K16" s="9">
-        <v>0</v>
-      </c>
-      <c r="L16" s="9">
-        <v>0</v>
-      </c>
-      <c r="M16" s="9">
-        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B17" s="9">
-        <v>253.42</v>
+        <v>582.83000000000004</v>
       </c>
       <c r="C17" s="9">
-        <v>0</v>
+        <v>571.09</v>
       </c>
       <c r="D17" s="9">
-        <v>0</v>
+        <v>134.13</v>
       </c>
       <c r="E17" s="9">
         <v>0</v>
@@ -3565,10 +3688,10 @@
     </row>
     <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="9">
-        <v>100</v>
+        <v>95.79</v>
       </c>
       <c r="C18" s="9">
         <v>0</v>
@@ -3606,598 +3729,639 @@
     </row>
     <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B19" s="9">
         <v>100</v>
       </c>
       <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="9">
         <v>100</v>
       </c>
-      <c r="D19" s="9">
+      <c r="C20" s="9">
         <v>100</v>
       </c>
-      <c r="E19" s="9">
+      <c r="D20" s="9">
         <v>100</v>
       </c>
-      <c r="F19" s="9">
+      <c r="E20" s="9">
         <v>100</v>
       </c>
-      <c r="G19" s="9">
+      <c r="F20" s="9">
         <v>100</v>
       </c>
-      <c r="H19" s="9">
+      <c r="G20" s="9">
         <v>100</v>
       </c>
-      <c r="I19" s="9">
+      <c r="H20" s="9">
         <v>100</v>
       </c>
-      <c r="J19" s="9">
+      <c r="I20" s="9">
         <v>100</v>
       </c>
-      <c r="K19" s="9">
+      <c r="J20" s="9">
         <v>100</v>
       </c>
-      <c r="L19" s="9">
+      <c r="K20" s="9">
         <v>100</v>
       </c>
-      <c r="M19" s="9">
+      <c r="L20" s="9">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="M20" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="9">
-        <v>0</v>
-      </c>
-      <c r="C20" s="9">
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9">
         <v>1500</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D21" s="9">
         <v>1500</v>
       </c>
-      <c r="E20" s="9">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0</v>
-      </c>
-      <c r="G20" s="9">
-        <v>0</v>
-      </c>
-      <c r="H20" s="9">
-        <v>0</v>
-      </c>
-      <c r="I20" s="9">
-        <v>0</v>
-      </c>
-      <c r="J20" s="9">
-        <v>0</v>
-      </c>
-      <c r="K20" s="9">
-        <v>0</v>
-      </c>
-      <c r="L20" s="9">
-        <v>0</v>
-      </c>
-      <c r="M20" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B22" s="9">
         <v>30</v>
       </c>
-      <c r="C21" s="9">
-        <v>0</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0</v>
-      </c>
-      <c r="E21" s="9">
-        <v>0</v>
-      </c>
-      <c r="F21" s="9">
-        <v>0</v>
-      </c>
-      <c r="G21" s="9">
-        <v>0</v>
-      </c>
-      <c r="H21" s="9">
-        <v>0</v>
-      </c>
-      <c r="I21" s="9">
-        <v>0</v>
-      </c>
-      <c r="J21" s="9">
-        <v>0</v>
-      </c>
-      <c r="K21" s="9">
-        <v>0</v>
-      </c>
-      <c r="L21" s="9">
-        <v>0</v>
-      </c>
-      <c r="M21" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
+      <c r="C22" s="9">
+        <v>0</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0</v>
+      </c>
+      <c r="M22" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="9">
-        <v>1400</v>
-      </c>
-      <c r="C23" s="9">
+      <c r="B24" s="9">
+        <v>1500</v>
+      </c>
+      <c r="C24" s="9">
         <v>200</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D24" s="9">
         <v>25500</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E24" s="9">
         <v>2300</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F24" s="9">
         <v>2200</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G24" s="9">
         <v>2200</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H24" s="9">
         <v>2200</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I24" s="9">
         <v>2200</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J24" s="9">
         <v>2200</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K24" s="9">
         <v>2200</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L24" s="9">
         <v>2200</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M24" s="9">
         <v>2300</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="9">
-        <v>0</v>
-      </c>
-      <c r="C24" s="9">
-        <v>0</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0</v>
-      </c>
-      <c r="F24" s="9">
-        <v>0</v>
-      </c>
-      <c r="G24" s="9">
-        <v>0</v>
-      </c>
-      <c r="H24" s="9">
-        <v>0</v>
-      </c>
-      <c r="I24" s="9">
-        <v>0</v>
-      </c>
-      <c r="J24" s="9">
-        <v>0</v>
-      </c>
-      <c r="K24" s="9">
-        <v>0</v>
-      </c>
-      <c r="L24" s="9">
-        <v>0</v>
-      </c>
-      <c r="M24" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="9">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9">
-        <v>0</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0</v>
-      </c>
-      <c r="E25" s="9">
-        <v>0</v>
-      </c>
-      <c r="F25" s="9">
-        <v>0</v>
-      </c>
-      <c r="G25" s="9">
-        <v>0</v>
-      </c>
-      <c r="H25" s="9">
-        <v>0</v>
-      </c>
-      <c r="I25" s="9">
-        <v>0</v>
-      </c>
-      <c r="J25" s="9">
-        <v>0</v>
-      </c>
-      <c r="K25" s="9">
-        <v>0</v>
-      </c>
-      <c r="L25" s="9">
-        <v>0</v>
-      </c>
-      <c r="M25" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="B26" s="9">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0</v>
+      </c>
+      <c r="L26" s="9">
+        <v>0</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="11">
-        <v>0</v>
-      </c>
-      <c r="C26" s="11">
-        <v>0</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0</v>
-      </c>
-      <c r="E26" s="11">
-        <v>0</v>
-      </c>
-      <c r="F26" s="11">
-        <v>0</v>
-      </c>
-      <c r="G26" s="11">
-        <v>0</v>
-      </c>
-      <c r="H26" s="11">
-        <v>0</v>
-      </c>
-      <c r="I26" s="11">
-        <v>0</v>
-      </c>
-      <c r="J26" s="11">
-        <v>0</v>
-      </c>
-      <c r="K26" s="11">
-        <v>0</v>
-      </c>
-      <c r="L26" s="11">
-        <v>0</v>
-      </c>
-      <c r="M26" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-    </row>
-    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+      <c r="B27" s="11">
+        <v>0</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0</v>
+      </c>
+      <c r="D27" s="11">
+        <v>0</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <v>0</v>
+      </c>
+      <c r="G27" s="11">
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
+        <v>0</v>
+      </c>
+      <c r="I27" s="11">
+        <v>0</v>
+      </c>
+      <c r="J27" s="11">
+        <v>0</v>
+      </c>
+      <c r="K27" s="11">
+        <v>0</v>
+      </c>
+      <c r="L27" s="11">
+        <v>0</v>
+      </c>
+      <c r="M27" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="10">
-        <f>SUM(B4:B5)-SUM(B7:B12)-SUM(B14:B21)-SUM(B23:B26)+B24+'2017'!M28</f>
-        <v>258.4700000000114</v>
-      </c>
-      <c r="C28" s="10">
-        <f t="shared" ref="C28:M28" si="0">SUM(C4:C5)-SUM(C7:C12)-SUM(C14:C21)-SUM(C23:C26)+B28+C24</f>
-        <v>213.2900000000111</v>
-      </c>
-      <c r="D28" s="10">
+      <c r="B29" s="10">
+        <f>SUM(B4:B6)-SUM(B8:B13)-SUM(B15:B22)-SUM(B24:B27)+'2017'!M29</f>
+        <v>276.10000000000548</v>
+      </c>
+      <c r="C29" s="10">
+        <f>SUM(C4:C6)-SUM(C8:C13)-SUM(C15:C22)-SUM(C24:C27)+B29</f>
+        <v>230.92000000000519</v>
+      </c>
+      <c r="D29" s="10">
+        <f t="shared" ref="D29:M29" si="0">SUM(D4:D6)-SUM(D8:D13)-SUM(D15:D22)-SUM(D24:D27)+C29</f>
+        <v>382.70000000000402</v>
+      </c>
+      <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>365.07000000000994</v>
-      </c>
-      <c r="E28" s="10">
+        <v>308.61000000000388</v>
+      </c>
+      <c r="F29" s="10">
         <f t="shared" si="0"/>
-        <v>290.9800000000098</v>
-      </c>
-      <c r="F28" s="10">
+        <v>334.52000000000373</v>
+      </c>
+      <c r="G29" s="10">
         <f t="shared" si="0"/>
-        <v>316.89000000000965</v>
-      </c>
-      <c r="G28" s="10">
+        <v>360.43000000000359</v>
+      </c>
+      <c r="H29" s="10">
         <f t="shared" si="0"/>
-        <v>342.8000000000095</v>
-      </c>
-      <c r="H28" s="10">
+        <v>386.34000000000344</v>
+      </c>
+      <c r="I29" s="10">
         <f t="shared" si="0"/>
-        <v>368.71000000000936</v>
-      </c>
-      <c r="I28" s="10">
+        <v>412.2500000000033</v>
+      </c>
+      <c r="J29" s="10">
         <f t="shared" si="0"/>
-        <v>394.62000000000921</v>
-      </c>
-      <c r="J28" s="10">
+        <v>438.16000000000315</v>
+      </c>
+      <c r="K29" s="10">
         <f t="shared" si="0"/>
-        <v>420.53000000000907</v>
-      </c>
-      <c r="K28" s="10">
+        <v>464.07000000000301</v>
+      </c>
+      <c r="L29" s="10">
         <f t="shared" si="0"/>
-        <v>446.44000000000892</v>
-      </c>
-      <c r="L28" s="10">
+        <v>489.98000000000286</v>
+      </c>
+      <c r="M29" s="10">
         <f t="shared" si="0"/>
-        <v>472.35000000000878</v>
-      </c>
-      <c r="M28" s="10">
-        <f t="shared" si="0"/>
-        <v>398.26000000000863</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
+        <v>415.89000000000271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="13">
-        <f>B23+'2017'!M29</f>
-        <v>6900</v>
-      </c>
-      <c r="C29" s="13">
-        <f t="shared" ref="C29:E29" si="1">C23+B29</f>
-        <v>7100</v>
-      </c>
-      <c r="D29" s="13">
+      <c r="B30" s="13">
+        <f>B24+'2017'!M30</f>
+        <v>49661.31</v>
+      </c>
+      <c r="C30" s="13">
+        <f t="shared" ref="C30:D30" si="1">C24+B30</f>
+        <v>49861.31</v>
+      </c>
+      <c r="D30" s="13">
         <f t="shared" si="1"/>
-        <v>32600</v>
-      </c>
-      <c r="E29" s="13">
-        <f t="shared" si="1"/>
-        <v>34900</v>
-      </c>
-      <c r="F29" s="13">
-        <f>F23+E29-F24</f>
-        <v>37100</v>
-      </c>
-      <c r="G29" s="13">
-        <f>G23+F29-G24</f>
-        <v>39300</v>
-      </c>
-      <c r="H29" s="13">
-        <f>H23+G29-H24</f>
-        <v>41500</v>
-      </c>
-      <c r="I29" s="13">
-        <f t="shared" ref="I29:M29" si="2">I23+H29-I24</f>
-        <v>43700</v>
-      </c>
-      <c r="J29" s="13">
+        <v>75361.31</v>
+      </c>
+      <c r="E30" s="13">
+        <f>E24+D30</f>
+        <v>77661.31</v>
+      </c>
+      <c r="F30" s="13">
+        <f>F24+E30-F25</f>
+        <v>79861.31</v>
+      </c>
+      <c r="G30" s="13">
+        <f>G24+F30-G25</f>
+        <v>82061.31</v>
+      </c>
+      <c r="H30" s="13">
+        <f>H24+G30-H25</f>
+        <v>84261.31</v>
+      </c>
+      <c r="I30" s="13">
+        <f t="shared" ref="I30:M30" si="2">I24+H30-I25</f>
+        <v>86461.31</v>
+      </c>
+      <c r="J30" s="13">
         <f t="shared" si="2"/>
-        <v>45900</v>
-      </c>
-      <c r="K29" s="13">
+        <v>88661.31</v>
+      </c>
+      <c r="K30" s="13">
         <f t="shared" si="2"/>
-        <v>48100</v>
-      </c>
-      <c r="L29" s="13">
+        <v>90861.31</v>
+      </c>
+      <c r="L30" s="13">
         <f t="shared" si="2"/>
-        <v>50300</v>
-      </c>
-      <c r="M29" s="13">
+        <v>93061.31</v>
+      </c>
+      <c r="M30" s="13">
         <f t="shared" si="2"/>
-        <v>52600</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+        <v>95361.31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="10">
-        <f t="shared" ref="B30:M30" si="3">B28+B29</f>
-        <v>7158.4700000000112</v>
-      </c>
-      <c r="C30" s="10">
+      <c r="B31" s="10">
+        <f t="shared" ref="B31:M31" si="3">B29+B30</f>
+        <v>49937.41</v>
+      </c>
+      <c r="C31" s="10">
         <f t="shared" si="3"/>
-        <v>7313.2900000000109</v>
-      </c>
-      <c r="D30" s="10">
+        <v>50092.23</v>
+      </c>
+      <c r="D31" s="10">
         <f t="shared" si="3"/>
-        <v>32965.070000000007</v>
-      </c>
-      <c r="E30" s="10">
+        <v>75744.009999999995</v>
+      </c>
+      <c r="E31" s="10">
         <f t="shared" si="3"/>
-        <v>35190.98000000001</v>
-      </c>
-      <c r="F30" s="10">
+        <v>77969.919999999998</v>
+      </c>
+      <c r="F31" s="10">
         <f t="shared" si="3"/>
-        <v>37416.890000000007</v>
-      </c>
-      <c r="G30" s="10">
+        <v>80195.83</v>
+      </c>
+      <c r="G31" s="10">
         <f t="shared" si="3"/>
-        <v>39642.80000000001</v>
-      </c>
-      <c r="H30" s="10">
+        <v>82421.740000000005</v>
+      </c>
+      <c r="H31" s="10">
         <f t="shared" si="3"/>
-        <v>41868.710000000006</v>
-      </c>
-      <c r="I30" s="10">
+        <v>84647.65</v>
+      </c>
+      <c r="I31" s="10">
         <f t="shared" si="3"/>
-        <v>44094.62000000001</v>
-      </c>
-      <c r="J30" s="10">
+        <v>86873.56</v>
+      </c>
+      <c r="J31" s="10">
         <f t="shared" si="3"/>
-        <v>46320.530000000006</v>
-      </c>
-      <c r="K30" s="10">
+        <v>89099.47</v>
+      </c>
+      <c r="K31" s="10">
         <f t="shared" si="3"/>
-        <v>48546.44000000001</v>
-      </c>
-      <c r="L30" s="10">
+        <v>91325.38</v>
+      </c>
+      <c r="L31" s="10">
         <f t="shared" si="3"/>
-        <v>50772.350000000006</v>
-      </c>
-      <c r="M30" s="10">
+        <v>93551.29</v>
+      </c>
+      <c r="M31" s="10">
         <f t="shared" si="3"/>
-        <v>52998.260000000009</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
+        <v>95777.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="H32" s="17">
+      <c r="H33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="I32" s="17">
+      <c r="I33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="J32" s="17">
+      <c r="J33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="K32" s="17">
+      <c r="K33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="L32" s="17">
+      <c r="L33" s="17">
         <v>268511.8</v>
       </c>
-      <c r="M32" s="17">
+      <c r="M33" s="17">
         <v>268511.8</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="G33" s="17">
+      <c r="G34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="H33" s="17">
+      <c r="H34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="I33" s="17">
+      <c r="I34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="J33" s="17">
+      <c r="J34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="K33" s="17">
+      <c r="K34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="L33" s="17">
+      <c r="L34" s="17">
         <v>212208.55</v>
       </c>
-      <c r="M33" s="17">
+      <c r="M34" s="17">
         <v>212208.55</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="G34" s="17">
+      <c r="G35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="H34" s="17">
+      <c r="H35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="L34" s="17">
+      <c r="L35" s="17">
         <v>150000.32000000001</v>
       </c>
-      <c r="M34" s="17">
+      <c r="M35" s="17">
         <v>150000.32000000001</v>
       </c>
     </row>

</xml_diff>